<commit_message>
updated ExtentReport files - Create customExtentSparkReport to create custom html report file instead of index.html
</commit_message>
<xml_diff>
--- a/Team7_Dollardays/target/classes/testdata.xlsx
+++ b/Team7_Dollardays/target/classes/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shachi\GitStuff\Dollardays\Team7_Dollardays\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6477B92-45CF-429C-8C51-9E145104B167}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141FDBCF-8468-4D16-B9A2-48753DD793A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="66">
   <si>
     <t>TCID</t>
   </si>
@@ -649,7 +649,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -706,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38EF0EC1-3A1B-4CD6-940E-FDAE6F9681BB}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1257,14 +1257,63 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{ABBF2275-28B6-4DF9-A8E4-B56A82CEF436}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Menu Items - TC1 -TC7 done
</commit_message>
<xml_diff>
--- a/Team7_Dollardays/target/classes/testdata.xlsx
+++ b/Team7_Dollardays/target/classes/testdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shachi\GitStuff\Dollardays\Team7_Dollardays\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141FDBCF-8468-4D16-B9A2-48753DD793A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF88AB07-0B99-4496-A563-852681DB339C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="106">
   <si>
     <t>TCID</t>
   </si>
@@ -221,13 +221,133 @@
   </si>
   <si>
     <t>Logged out from Account web page.</t>
+  </si>
+  <si>
+    <t>Validate Menu Items - Main Categories</t>
+  </si>
+  <si>
+    <t>Validate Sorting - Sort by 'Alphabetically by Name'</t>
+  </si>
+  <si>
+    <t>Add an item to cart without login</t>
+  </si>
+  <si>
+    <t>Search an item through ShopAll button  in Menu and add to the cart</t>
+  </si>
+  <si>
+    <t>Add an Item from SubCategories to the cart through Menu</t>
+  </si>
+  <si>
+    <t>Add an item from categories to the cart through Menu</t>
+  </si>
+  <si>
+    <t>Validate paging on item lists</t>
+  </si>
+  <si>
+    <t>Total 4 Categories-Now Trending,Categories,Programs,Help &amp; Settings</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Reflective Dog Collar - 14"-22" - Assorted Colors</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 15" Forward Classic School Backpack with Side Mesh Pocket - 8 Colors</t>
+  </si>
+  <si>
+    <t>Items are sorted in Alphabetically order by name</t>
+  </si>
+  <si>
+    <t>Select total number of items which should display per page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of items displayed as per selected number in 'View' dropdown </t>
+  </si>
+  <si>
+    <t>No of Item per Page</t>
+  </si>
+  <si>
+    <t>Paging</t>
+  </si>
+  <si>
+    <t>Alphabetically by Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paging is working </t>
+  </si>
+  <si>
+    <t>It navigates to Login page when click on 'Login to Buy' button below item name in item list page</t>
+  </si>
+  <si>
+    <t>Verify Categories</t>
+  </si>
+  <si>
+    <t>Baby-&gt;Bedding &amp; Blankets</t>
+  </si>
+  <si>
+    <t>Food-&gt;Coffee, Tea &amp; Cocoa-&gt;Cocoa</t>
+  </si>
+  <si>
+    <t>SortItem</t>
+  </si>
+  <si>
+    <t>ExpectedResult</t>
+  </si>
+  <si>
+    <t>Item flow</t>
+  </si>
+  <si>
+    <t>Pet Supplies-&gt;Dog Supplies-&gt;Shop All</t>
+  </si>
+  <si>
+    <t>Pet Supplies-&gt;Shop All</t>
+  </si>
+  <si>
+    <t>TargetURL</t>
+  </si>
+  <si>
+    <t>https://www.dollardays.com/wholesale-pet-treats-and-essentials.html</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>isItemAddedtoCart</t>
+  </si>
+  <si>
+    <t>Product is added to cart</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Baby Gingahm Blanket with Embroidery - Pink &amp; Blue</t>
+  </si>
+  <si>
+    <t>https://www.dollardays.com/wholesale-baby-bedding.html</t>
+  </si>
+  <si>
+    <t>https://www.dollardays.com/wholesale-backpacks.html</t>
+  </si>
+  <si>
+    <t>For Educators-&gt;Backpacks-link on web page</t>
+  </si>
+  <si>
+    <t>https://www.dollardays.com/wholesale-hot-cocoa.html</t>
+  </si>
+  <si>
+    <t>https://www.dollardays.com/wholesale-blankets-and-throws.html</t>
+  </si>
+  <si>
+    <t>Bedding, Bath &amp; Decor-&gt; Blankets &amp; Bedding-&gt; Blankets &amp; Throws</t>
+  </si>
+  <si>
+    <t>24,12,48</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,6 +374,12 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -286,7 +412,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -306,6 +432,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1257,23 +1386,30 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" customWidth="1"/>
+    <col min="2" max="2" width="67.6640625" customWidth="1"/>
     <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.21875" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="81.44140625" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" customWidth="1"/>
+    <col min="8" max="8" width="16.21875" customWidth="1"/>
+    <col min="9" max="10" width="54.33203125" customWidth="1"/>
+    <col min="11" max="11" width="57.77734375" customWidth="1"/>
+    <col min="12" max="12" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.5546875" customWidth="1"/>
+    <col min="14" max="14" width="7.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1290,29 +1426,274 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
+      <c r="B2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" t="s">
+        <v>91</v>
+      </c>
+      <c r="J3" t="s">
+        <v>94</v>
+      </c>
+      <c r="K3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" t="s">
+        <v>86</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="K4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" t="s">
+        <v>101</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="K5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" t="s">
+        <v>87</v>
+      </c>
+      <c r="J6" t="s">
+        <v>102</v>
+      </c>
+      <c r="L6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>79</v>
+      </c>
+      <c r="I7" t="s">
+        <v>104</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>83</v>
+      </c>
+      <c r="I8" t="s">
+        <v>104</v>
+      </c>
+      <c r="J8" t="s">
+        <v>103</v>
+      </c>
+      <c r="M8" s="10">
+        <v>24</v>
+      </c>
+      <c r="N8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>84</v>
+      </c>
+      <c r="I9" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{ABBF2275-28B6-4DF9-A8E4-B56A82CEF436}"/>
+    <hyperlink ref="D3:D9" r:id="rId2" display="srikanthtesting100@gmail.com" xr:uid="{7B63AB3A-32FF-4BC1-B8AC-EB01D3B1D4CF}"/>
+    <hyperlink ref="J4" r:id="rId3" xr:uid="{E84440EF-2B98-49B7-9B62-52DAEBD8396A}"/>
+    <hyperlink ref="J5" r:id="rId4" xr:uid="{1CB006B1-729E-47C1-A819-0A42563CA166}"/>
+    <hyperlink ref="J7" r:id="rId5" xr:uid="{633D32D6-D541-45A6-B5F2-27D131BC09D4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Menu Test Case - done
</commit_message>
<xml_diff>
--- a/Team7_Dollardays/target/classes/testdata.xlsx
+++ b/Team7_Dollardays/target/classes/testdata.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shachi\GitStuff\Dollardays\Team7_Dollardays\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF88AB07-0B99-4496-A563-852681DB339C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A09C5EB-3FC3-4C0D-93ED-D77C5A8E9AED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Logout" sheetId="4" r:id="rId2"/>
     <sheet name="SubmitRequest" sheetId="2" r:id="rId3"/>
     <sheet name="Menu" sheetId="3" r:id="rId4"/>
+    <sheet name="Search" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="141">
   <si>
     <t>TCID</t>
   </si>
@@ -247,9 +248,6 @@
     <t>Total 4 Categories-Now Trending,Categories,Programs,Help &amp; Settings</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Reflective Dog Collar - 14"-22" - Assorted Colors</t>
   </si>
   <si>
@@ -277,9 +275,6 @@
     <t xml:space="preserve">Paging is working </t>
   </si>
   <si>
-    <t>It navigates to Login page when click on 'Login to Buy' button below item name in item list page</t>
-  </si>
-  <si>
     <t>Verify Categories</t>
   </si>
   <si>
@@ -341,6 +336,123 @@
   </si>
   <si>
     <t>24,12,48</t>
+  </si>
+  <si>
+    <t>AddItemWithoutLogin</t>
+  </si>
+  <si>
+    <t>https://www.dollardays.com/wholesale-pets.html</t>
+  </si>
+  <si>
+    <t>Pet Pedicure Tool</t>
+  </si>
+  <si>
+    <t>navigated to Login page when click on 'Login to Buy' button below item name in item list page</t>
+  </si>
+  <si>
+    <t>VerifyDefaultSearchResult - Click on an item in Default 'Search Results' window,It should display related product item list page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. On Clicking in 'Search' field, Default 'Search Result' box is displayed.
+2. RightPane has 'Now Trending' product item list
+3. Left pane has popular product categories list titled 'Popular categories' 
+4. Clicking on a product in right pane, navigated to  product Item Page  </t>
+  </si>
+  <si>
+    <t>blankets throws;kn95;adult coloring books</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>Leftpane Category</t>
+  </si>
+  <si>
+    <t>kn95</t>
+  </si>
+  <si>
+    <t>VerifyLeftPaneMouseHover-  item list should be updated when Mousehover on item list in left pane</t>
+  </si>
+  <si>
+    <t>Folding Cell Phone Stand</t>
+  </si>
+  <si>
+    <t>Product item is listed in 'Search Result' window and on clicking , it is navigated to 'Item detail' page</t>
+  </si>
+  <si>
+    <t>https://www.dollardays.com/i2182286-wholesale-folding-cell-phone-stand.html</t>
+  </si>
+  <si>
+    <t>VerifyShowMoreProductsClick</t>
+  </si>
+  <si>
+    <t>1. releted product items are listed in 'Search Result' alond with 'Show more products' button.
+2. item page is displayed on clicking on 'Show More Products' 
+3. Product search text is displayed in 'Search' field</t>
+  </si>
+  <si>
+    <t>notebook</t>
+  </si>
+  <si>
+    <t>https://www.dollardays.com/sitesearch.aspx?pg=1&amp;terms=notebook</t>
+  </si>
+  <si>
+    <t>Product item list getting updated in right pane in 'Search Result' box and product title contains text of Category name</t>
+  </si>
+  <si>
+    <t>Clicked item is displayed in 'Search' field and related product item list page is displayed.</t>
+  </si>
+  <si>
+    <t>https://www.dollardays.com/sitesearch.aspx?pg=1&amp;terms=kn95</t>
+  </si>
+  <si>
+    <t>SearchItem</t>
+  </si>
+  <si>
+    <t>VerifySearchField-Enter item in 'Search Field' then click on sub category from 'Did you Mean' left pane</t>
+  </si>
+  <si>
+    <t>1.Related item is displayed in 'Search Result' pane 
+2.Clicked item is displayed in 'Search' field and related product item list page is displayed.</t>
+  </si>
+  <si>
+    <t>cell phone</t>
+  </si>
+  <si>
+    <t>https://www.dollardays.com/sitesearch.aspx?pg=1&amp;terms=cell%20phone</t>
+  </si>
+  <si>
+    <t>VerifySearchField-Open item detail page by passing full Product name in search field and clicking on item in 'Search Result' box.</t>
+  </si>
+  <si>
+    <t>backpack</t>
+  </si>
+  <si>
+    <t>https://www.dollardays.com/sitesearch.aspx?pg=1&amp;terms=backpack</t>
+  </si>
+  <si>
+    <t>searchPageWithNavigationLinks</t>
+  </si>
+  <si>
+    <t>searchWithValidData</t>
+  </si>
+  <si>
+    <t>searchWithInvalidDta</t>
+  </si>
+  <si>
+    <t>blurkdfhdkhsdfresadsa</t>
+  </si>
+  <si>
+    <t>https://www.dollardays.com/sitesearch.aspx?pg=1&amp;terms=blurkdfhdkhsdfresadsa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Item Page is displayed </t>
+  </si>
+  <si>
+    <t>No Results Found for "blurkdfhdkhsdfresadsa"</t>
+  </si>
+  <si>
+    <t>VerifyLeftPaneItemClick - Category name should display in 'Search' field and  related product item list page should be open.</t>
   </si>
 </sst>
 </file>
@@ -412,7 +524,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -433,8 +545,18 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1386,10 +1508,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1405,11 +1527,12 @@
     <col min="9" max="10" width="54.33203125" customWidth="1"/>
     <col min="11" max="11" width="57.77734375" customWidth="1"/>
     <col min="12" max="12" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.5546875" customWidth="1"/>
+    <col min="13" max="13" width="19.5546875" style="13" customWidth="1"/>
     <col min="14" max="14" width="7.44140625" customWidth="1"/>
+    <col min="15" max="15" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1426,34 +1549,37 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="M1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O1" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -1476,8 +1602,9 @@
       <c r="H2" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M2" s="12"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1494,22 +1621,22 @@
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G3" t="s">
         <v>6</v>
       </c>
       <c r="I3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1526,22 +1653,22 @@
         <v>8</v>
       </c>
       <c r="F4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" t="s">
+        <v>84</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="G4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" t="s">
-        <v>86</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>99</v>
-      </c>
       <c r="K4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1558,22 +1685,22 @@
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G5" t="s">
         <v>6</v>
       </c>
       <c r="I5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1590,48 +1717,48 @@
         <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="L6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
       <c r="B7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" t="s">
-        <v>79</v>
-      </c>
       <c r="I7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J7" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="M7" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="M7" s="10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1639,7 +1766,7 @@
         <v>72</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>74</v>
+        <v>6</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>7</v>
@@ -1648,22 +1775,22 @@
         <v>8</v>
       </c>
       <c r="F8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="M8" s="10">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="N8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1671,7 +1798,7 @@
         <v>68</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>74</v>
+        <v>6</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>7</v>
@@ -1680,10 +1807,19 @@
         <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>84</v>
+        <v>107</v>
       </c>
       <c r="I9" t="s">
-        <v>92</v>
+        <v>90</v>
+      </c>
+      <c r="J9" t="s">
+        <v>105</v>
+      </c>
+      <c r="K9" t="s">
+        <v>106</v>
+      </c>
+      <c r="O9" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1696,5 +1832,301 @@
     <hyperlink ref="J7" r:id="rId5" xr:uid="{633D32D6-D541-45A6-B5F2-27D131BC09D4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FA6042B-23B9-44A7-A318-A0D1B2DCE5F5}">
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="108" customWidth="1"/>
+    <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="102.88671875" customWidth="1"/>
+    <col min="7" max="7" width="68.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="68" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G2" t="s">
+        <v>131</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G3" t="s">
+        <v>136</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G4" t="s">
+        <v>131</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="6" customFormat="1" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>123</v>
+      </c>
+      <c r="H7" t="s">
+        <v>113</v>
+      </c>
+      <c r="I7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>116</v>
+      </c>
+      <c r="G8" t="s">
+        <v>115</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="6" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{5D72B205-44DB-4023-A845-2A3EA27A6EA7}"/>
+    <hyperlink ref="I8" r:id="rId2" xr:uid="{0D5B46F7-37AC-4EBD-A98C-7AAE95A64114}"/>
+    <hyperlink ref="D8" r:id="rId3" xr:uid="{4ECD9683-7C72-4F96-8992-54B34A217E5B}"/>
+    <hyperlink ref="I9" r:id="rId4" xr:uid="{EA008E56-0655-4C44-B3C9-F98067AF16F7}"/>
+    <hyperlink ref="I4" r:id="rId5" xr:uid="{5E34FCD1-6F45-43E0-B9B9-330763D76ABE}"/>
+    <hyperlink ref="I2" r:id="rId6" xr:uid="{5C327096-0E97-44DD-9BE8-F8D85BADFB62}"/>
+    <hyperlink ref="I3" r:id="rId7" xr:uid="{3AE9FDB5-C7DF-4BE8-9CD4-1E6DA0478C52}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Feb9th - Search Page Automation
</commit_message>
<xml_diff>
--- a/Team7_Dollardays/target/classes/testdata.xlsx
+++ b/Team7_Dollardays/target/classes/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shachi\GitStuff\Dollardays\Team7_Dollardays\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C1381D-1856-4B4C-AB6E-E54A913D24DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D2B8D9B-C392-47CE-AE5D-4042E1772D5B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -203,9 +203,6 @@
     <t>Missing item(s)</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>Submit A Request</t>
   </si>
   <si>
@@ -359,9 +356,6 @@
 4. Clicking on a product in right pane, navigated to  product Item Page  </t>
   </si>
   <si>
-    <t>blankets throws;kn95;adult coloring books</t>
-  </si>
-  <si>
     <t>phone</t>
   </si>
   <si>
@@ -453,6 +447,12 @@
   </si>
   <si>
     <t>VerifyLeftPaneItemClick - Category name should display in 'Search' field and  related product item list page should be open.</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Wipes;kn95;N95</t>
   </si>
 </sst>
 </file>
@@ -986,7 +986,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -994,7 +994,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -1006,7 +1006,7 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1014,7 +1014,7 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -1026,7 +1026,7 @@
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1042,8 +1042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1161,7 +1161,7 @@
         <v>8</v>
       </c>
       <c r="L3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P3" t="s">
         <v>41</v>
@@ -1281,7 +1281,7 @@
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>7</v>
@@ -1308,7 +1308,7 @@
         <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>7</v>
@@ -1337,7 +1337,7 @@
         <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>7</v>
@@ -1369,7 +1369,7 @@
         <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>7</v>
@@ -1401,7 +1401,7 @@
         <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>7</v>
@@ -1427,7 +1427,7 @@
         <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>7</v>
@@ -1453,7 +1453,7 @@
         <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>7</v>
@@ -1476,7 +1476,7 @@
         <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>7</v>
@@ -1511,7 +1511,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1549,34 +1549,34 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M1" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="O1" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -1584,7 +1584,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>6</v>
@@ -1596,7 +1596,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5" t="s">
@@ -1609,7 +1609,7 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>6</v>
@@ -1621,19 +1621,19 @@
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G3" t="s">
         <v>6</v>
       </c>
       <c r="I3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -1641,7 +1641,7 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>6</v>
@@ -1653,19 +1653,19 @@
         <v>8</v>
       </c>
       <c r="F4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" t="s">
+        <v>83</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K4" t="s">
         <v>95</v>
-      </c>
-      <c r="G4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" t="s">
-        <v>84</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="K4" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -1673,7 +1673,7 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>6</v>
@@ -1685,19 +1685,19 @@
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G5" t="s">
         <v>6</v>
       </c>
       <c r="I5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -1705,7 +1705,7 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>6</v>
@@ -1717,16 +1717,16 @@
         <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -1734,28 +1734,28 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
         <v>77</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" t="s">
-        <v>78</v>
-      </c>
       <c r="I7" t="s">
+        <v>101</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="M7" s="10" t="s">
         <v>102</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="M7" s="10" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -1763,7 +1763,7 @@
         <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>6</v>
@@ -1775,13 +1775,13 @@
         <v>8</v>
       </c>
       <c r="F8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M8" s="10">
         <v>12</v>
@@ -1795,7 +1795,7 @@
         <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>6</v>
@@ -1807,16 +1807,16 @@
         <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J9" t="s">
+        <v>104</v>
+      </c>
+      <c r="K9" t="s">
         <v>105</v>
-      </c>
-      <c r="K9" t="s">
-        <v>106</v>
       </c>
       <c r="O9" t="s">
         <v>6</v>
@@ -1841,7 +1841,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1875,16 +1875,16 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J1" s="1"/>
     </row>
@@ -1893,10 +1893,10 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>6</v>
+        <v>139</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>7</v>
@@ -1905,13 +1905,13 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1919,25 +1919,25 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>137</v>
+      </c>
+      <c r="G3" t="s">
+        <v>134</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>135</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" t="s">
-        <v>139</v>
-      </c>
-      <c r="G3" t="s">
-        <v>136</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -1945,10 +1945,10 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>6</v>
+        <v>139</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>7</v>
@@ -1957,13 +1957,13 @@
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="6" customFormat="1" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1971,19 +1971,19 @@
         <v>18</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>108</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -1991,7 +1991,7 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>6</v>
@@ -2003,10 +2003,10 @@
         <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H6" t="s">
-        <v>110</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -2014,7 +2014,7 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>6</v>
@@ -2026,13 +2026,13 @@
         <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -2040,7 +2040,7 @@
         <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>6</v>
@@ -2052,13 +2052,13 @@
         <v>8</v>
       </c>
       <c r="F8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G8" t="s">
+        <v>113</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>115</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -2066,28 +2066,28 @@
         <v>29</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="H9" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="5" t="s">
+      <c r="I9" s="14" t="s">
         <v>127</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="6" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -2095,25 +2095,25 @@
         <v>30</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="G10" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="5" t="s">
+      <c r="I10" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>